<commit_message>
update WGCNA overlapped genes
</commit_message>
<xml_diff>
--- a/RAnalysis/Output/Water_Chem/Chem.Table_forMS.xlsx
+++ b/RAnalysis/Output/Water_Chem/Chem.Table_forMS.xlsx
@@ -1,27 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\samjg\Documents\Github_repositories\Cvirginica_multistressor\RAnalysis\Output\Water_Chem\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{EA6C1B4C-115D-4D35-B247-C0A19D84AB12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDB30BFB-C492-45E5-A15F-57D6955CDE02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14955" yWindow="-16320" windowWidth="29040" windowHeight="15720" activeTab="1"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Chem.Table_forMS" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="295" uniqueCount="229">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="395" uniqueCount="266">
   <si>
     <t>temp</t>
   </si>
@@ -763,11 +764,128 @@
       <t>3</t>
     </r>
   </si>
+  <si>
+    <t>Shannon 12/13/2022 :"Salinity= 2 decimals
+pco2=good
+Temperature=1 decimal
+pH= 4 decimals
+REmove HCO3 and CO3 from the table please
+TA= 2 decimal
+Aragonite= 2 decimal"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">17.25 ± 0.051 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">17.38 ± 0.065 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">17.27 ± 0.047 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">27.36 ± 0.051 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">17.40 ± 0.055 </t>
+  </si>
+  <si>
+    <t>27.56 ± 0.069</t>
+  </si>
+  <si>
+    <t xml:space="preserve">27.30 ± 0.044 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">27.56 ± 0.056 </t>
+  </si>
+  <si>
+    <t>23.0 ± 0.1</t>
+  </si>
+  <si>
+    <t>27.1 ± 0.1</t>
+  </si>
+  <si>
+    <t>27.0 ± 0.1</t>
+  </si>
+  <si>
+    <t>23.1 ± 0.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7.2563 ± 0.0055 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">7.2807 ± 0.012 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">7.6460 ± 0.0043 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">7.6618 ± 0.0052 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">7.4036 ± 0.0052 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">7.4072 ± 0.0055 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">7.8019 ± 0.0029 </t>
+  </si>
+  <si>
+    <t>7.8018 ± 0.0043</t>
+  </si>
+  <si>
+    <t>1258.86 ± 12.79</t>
+  </si>
+  <si>
+    <t>1268.84 ± 10.92</t>
+  </si>
+  <si>
+    <t>1931.49 ± 7.25</t>
+  </si>
+  <si>
+    <t>1943.57 ± 10.81</t>
+  </si>
+  <si>
+    <t>1969.48 ± 8.14</t>
+  </si>
+  <si>
+    <t>1977.31 ± 6.79</t>
+  </si>
+  <si>
+    <t>1259.68 ± 5.44</t>
+  </si>
+  <si>
+    <t>1256.78 ± 19.70</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.9 ± 0.03 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.5 ± 0.02 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.78 ± 0.01 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.66 ± 0.01 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.67 ± 0.01 </t>
+  </si>
+  <si>
+    <t>0.55 ± 0.01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.30 ± 0.01 </t>
+  </si>
+  <si>
+    <t>0.23 ± 0.004</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="23" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1287,7 +1405,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1313,6 +1431,9 @@
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -1668,7 +1789,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:L27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2275,11 +2396,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B2:N18"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView showGridLines="0" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2789,4 +2910,456 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E7A2B5E-8DBC-4BFF-A27E-3FDF6FC5A7F7}">
+  <dimension ref="B2:L26"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="L8" sqref="L8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="4" width="13.90625" customWidth="1"/>
+    <col min="5" max="5" width="14.36328125" customWidth="1"/>
+    <col min="7" max="8" width="18.81640625" customWidth="1"/>
+    <col min="9" max="9" width="18.81640625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="19.6328125" style="1" customWidth="1"/>
+    <col min="11" max="11" width="21.7265625" style="1" customWidth="1"/>
+    <col min="12" max="12" width="18.81640625" style="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:12" ht="4" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="3"/>
+      <c r="J2" s="3"/>
+      <c r="K2" s="3"/>
+      <c r="L2" s="3"/>
+    </row>
+    <row r="3" spans="2:12" ht="18" x14ac:dyDescent="0.4">
+      <c r="B3" s="5" t="s">
+        <v>152</v>
+      </c>
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="5" t="s">
+        <v>154</v>
+      </c>
+      <c r="G3" s="6"/>
+      <c r="H3" s="6"/>
+      <c r="I3" s="7"/>
+      <c r="J3" s="7"/>
+      <c r="K3" s="7"/>
+      <c r="L3" s="7"/>
+    </row>
+    <row r="4" spans="2:12" ht="5.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B4" s="6"/>
+      <c r="C4" s="6"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="6"/>
+      <c r="G4" s="6"/>
+      <c r="H4" s="6"/>
+      <c r="I4" s="7"/>
+      <c r="J4" s="7"/>
+      <c r="K4" s="7"/>
+      <c r="L4" s="7"/>
+    </row>
+    <row r="5" spans="2:12" ht="20.5" x14ac:dyDescent="0.5">
+      <c r="B5" s="6"/>
+      <c r="C5" s="6"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="6"/>
+      <c r="F5" s="6"/>
+      <c r="G5" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="H5" s="8" t="s">
+        <v>226</v>
+      </c>
+      <c r="I5" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="J5" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="K5" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="L5" s="7" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="6" spans="2:12" ht="20.5" x14ac:dyDescent="0.5">
+      <c r="B6" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>226</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>153</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>159</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>160</v>
+      </c>
+      <c r="I6" s="4" t="s">
+        <v>225</v>
+      </c>
+      <c r="J6" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="K6" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="L6" s="7" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="7" spans="2:12" ht="5.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B7" s="6"/>
+      <c r="C7" s="6"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="6"/>
+      <c r="G7" s="6"/>
+      <c r="H7" s="6"/>
+      <c r="I7" s="7"/>
+      <c r="J7" s="7"/>
+      <c r="K7" s="7"/>
+      <c r="L7" s="7"/>
+    </row>
+    <row r="8" spans="2:12" ht="5.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B8" s="9"/>
+      <c r="C8" s="9"/>
+      <c r="D8" s="9"/>
+      <c r="E8" s="9"/>
+      <c r="F8" s="9"/>
+      <c r="G8" s="9"/>
+      <c r="H8" s="9"/>
+      <c r="I8" s="10"/>
+      <c r="J8" s="10"/>
+      <c r="K8" s="10"/>
+      <c r="L8" s="10"/>
+    </row>
+    <row r="9" spans="2:12" s="1" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B9" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="F9" s="7">
+        <v>14</v>
+      </c>
+      <c r="G9" s="7" t="s">
+        <v>230</v>
+      </c>
+      <c r="H9" s="7" t="s">
+        <v>218</v>
+      </c>
+      <c r="I9" s="7" t="s">
+        <v>238</v>
+      </c>
+      <c r="J9" s="7" t="s">
+        <v>242</v>
+      </c>
+      <c r="K9" s="7" t="s">
+        <v>250</v>
+      </c>
+      <c r="L9" s="7" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="10" spans="2:12" s="1" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B10" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="E10" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="F10" s="7">
+        <v>16</v>
+      </c>
+      <c r="G10" s="7" t="s">
+        <v>231</v>
+      </c>
+      <c r="H10" s="7" t="s">
+        <v>171</v>
+      </c>
+      <c r="I10" s="7" t="s">
+        <v>239</v>
+      </c>
+      <c r="J10" s="7" t="s">
+        <v>243</v>
+      </c>
+      <c r="K10" s="7" t="s">
+        <v>251</v>
+      </c>
+      <c r="L10" s="7" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="11" spans="2:12" s="1" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B11" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="F11" s="7">
+        <v>18</v>
+      </c>
+      <c r="G11" s="7" t="s">
+        <v>232</v>
+      </c>
+      <c r="H11" s="7" t="s">
+        <v>210</v>
+      </c>
+      <c r="I11" s="7" t="s">
+        <v>238</v>
+      </c>
+      <c r="J11" s="7" t="s">
+        <v>244</v>
+      </c>
+      <c r="K11" s="7" t="s">
+        <v>257</v>
+      </c>
+      <c r="L11" s="7" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="12" spans="2:12" s="1" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B12" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="E12" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="F12" s="7">
+        <v>18</v>
+      </c>
+      <c r="G12" s="7" t="s">
+        <v>234</v>
+      </c>
+      <c r="H12" s="7" t="s">
+        <v>186</v>
+      </c>
+      <c r="I12" s="7" t="s">
+        <v>240</v>
+      </c>
+      <c r="J12" s="7" t="s">
+        <v>245</v>
+      </c>
+      <c r="K12" s="7" t="s">
+        <v>256</v>
+      </c>
+      <c r="L12" s="7" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="13" spans="2:12" s="1" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B13" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="E13" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="F13" s="7">
+        <v>18</v>
+      </c>
+      <c r="G13" s="7" t="s">
+        <v>233</v>
+      </c>
+      <c r="H13" s="7" t="s">
+        <v>194</v>
+      </c>
+      <c r="I13" s="7" t="s">
+        <v>241</v>
+      </c>
+      <c r="J13" s="7" t="s">
+        <v>246</v>
+      </c>
+      <c r="K13" s="7" t="s">
+        <v>255</v>
+      </c>
+      <c r="L13" s="7" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="14" spans="2:12" s="1" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B14" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="E14" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="F14" s="7">
+        <v>18</v>
+      </c>
+      <c r="G14" s="11" t="s">
+        <v>235</v>
+      </c>
+      <c r="H14" s="11" t="s">
+        <v>165</v>
+      </c>
+      <c r="I14" s="11" t="s">
+        <v>239</v>
+      </c>
+      <c r="J14" s="11" t="s">
+        <v>247</v>
+      </c>
+      <c r="K14" s="7" t="s">
+        <v>254</v>
+      </c>
+      <c r="L14" s="7" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="15" spans="2:12" s="1" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B15" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D15" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="E15" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="F15" s="7">
+        <v>18</v>
+      </c>
+      <c r="G15" s="7" t="s">
+        <v>236</v>
+      </c>
+      <c r="H15" s="7" t="s">
+        <v>202</v>
+      </c>
+      <c r="I15" s="7" t="s">
+        <v>241</v>
+      </c>
+      <c r="J15" s="7" t="s">
+        <v>248</v>
+      </c>
+      <c r="K15" s="7" t="s">
+        <v>253</v>
+      </c>
+      <c r="L15" s="7" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="16" spans="2:12" s="1" customFormat="1" ht="23" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B16" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D16" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="E16" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="F16" s="7">
+        <v>18</v>
+      </c>
+      <c r="G16" s="7" t="s">
+        <v>237</v>
+      </c>
+      <c r="H16" s="7" t="s">
+        <v>178</v>
+      </c>
+      <c r="I16" s="7" t="s">
+        <v>239</v>
+      </c>
+      <c r="J16" s="7" t="s">
+        <v>249</v>
+      </c>
+      <c r="K16" s="7" t="s">
+        <v>252</v>
+      </c>
+      <c r="L16" s="7" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="17" spans="2:12" ht="4" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="18" spans="2:12" x14ac:dyDescent="0.35">
+      <c r="B18" s="2"/>
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="2"/>
+      <c r="G18" s="2"/>
+      <c r="H18" s="2"/>
+      <c r="I18" s="3"/>
+      <c r="J18" s="3"/>
+      <c r="K18" s="3"/>
+      <c r="L18" s="3"/>
+    </row>
+    <row r="26" spans="2:12" ht="217.5" x14ac:dyDescent="0.35">
+      <c r="B26" s="12" t="s">
+        <v>229</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>